<commit_message>
Even more new stuff
</commit_message>
<xml_diff>
--- a/testfile.xlsx
+++ b/testfile.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>sdfds</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>sdfdsfsd</t>
+  </si>
+  <si>
+    <t>sdfdsfsdf</t>
   </si>
 </sst>
 </file>
@@ -378,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:O23"/>
+  <dimension ref="B3:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,14 +419,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
       <c r="O23" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New stuff from reverted version
</commit_message>
<xml_diff>
--- a/testfile.xlsx
+++ b/testfile.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>sdfds</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>sdfdsfsd</t>
+  </si>
+  <si>
+    <t>sfdsfsd</t>
+  </si>
+  <si>
+    <t>sfdsfs</t>
   </si>
 </sst>
 </file>
@@ -378,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:O23"/>
+  <dimension ref="B3:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,14 +422,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="P20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="L22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
       <c r="O23" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>